<commit_message>
Popravljen ispis kvara sa prioritetom
</commit_message>
<xml_diff>
--- a/OMS/OMS/bin/Debug/oms.xlsx
+++ b/OMS/OMS/bin/Debug/oms.xlsx
@@ -173,6 +173,15 @@
   </x:si>
   <x:si>
     <x:t>Novi opis duzi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20240104084543_01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024-01-04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Radni se</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -523,7 +532,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F12"/>
+  <x:dimension ref="A1:F13"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -769,6 +778,26 @@
         <x:v>27</x:v>
       </x:c>
     </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>